<commit_message>
invitee import password field added
</commit_message>
<xml_diff>
--- a/public/invitee_sample.xlsx
+++ b/public/invitee_sample.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>email</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>facebook_link</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
   <si>
     <t>invitee@example.com</t>
@@ -190,10 +193,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -247,43 +250,49 @@
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>9876543210</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
invitee import and export social links added
</commit_message>
<xml_diff>
--- a/public/invitee_sample.xlsx
+++ b/public/invitee_sample.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>email</t>
   </si>
@@ -55,6 +55,12 @@
     <t>facebook_link</t>
   </si>
   <si>
+    <t>google+_link</t>
+  </si>
+  <si>
+    <t>linkedin_link</t>
+  </si>
+  <si>
     <t>password</t>
   </si>
   <si>
@@ -86,6 +92,9 @@
   </si>
   <si>
     <t>Coolshiv@facebook.com</t>
+  </si>
+  <si>
+    <t>Coolshiv@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -193,9 +202,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -253,46 +262,58 @@
       <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>9876543210</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>12</v>
+        <v>25</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
invitee import and export profile pic url added
</commit_message>
<xml_diff>
--- a/public/invitee_sample.xlsx
+++ b/public/invitee_sample.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>email</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>Profile picture</t>
   </si>
   <si>
     <t>invitee@example.com</t>
@@ -202,10 +205,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -268,49 +271,52 @@
       <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>9876543210</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O2" s="0" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
invitee import and export field name change and agenda set_time method changes
</commit_message>
<xml_diff>
--- a/public/invitee_sample.xlsx
+++ b/public/invitee_sample.xlsx
@@ -64,7 +64,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>Profile picture</t>
+    <t>Profile_pic_URL</t>
   </si>
   <si>
     <t>invitee@example.com</t>
@@ -208,7 +208,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
merging remark_field_added_in_invitee_model into staging
</commit_message>
<xml_diff>
--- a/public/invitee_sample.xlsx
+++ b/public/invitee_sample.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>email</t>
   </si>
@@ -64,7 +64,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>Profile_pic_URL</t>
+    <t>Profile picture</t>
+  </si>
+  <si>
+    <t>Remark</t>
   </si>
   <si>
     <t>invitee@example.com</t>
@@ -205,10 +208,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -274,49 +277,52 @@
       <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>9876543210</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O2" s="0" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
invitee remark field added and remove validation of mobile no in speaker
</commit_message>
<xml_diff>
--- a/public/invitee_sample.xlsx
+++ b/public/invitee_sample.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>email</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Profile picture</t>
+  </si>
+  <si>
+    <t>Remark</t>
   </si>
   <si>
     <t>invitee@example.com</t>
@@ -205,10 +208,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -274,49 +277,52 @@
       <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>9876543210</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O2" s="0" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
field added in form, import, export
</commit_message>
<xml_diff>
--- a/public/invitee_sample.xlsx
+++ b/public/invitee_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="176" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="170" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>email</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>linkedin_link</t>
+  </si>
+  <si>
+    <t>instagram</t>
   </si>
   <si>
     <t>password</t>
@@ -110,7 +113,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -138,6 +141,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -182,12 +191,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -208,10 +221,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -280,58 +293,65 @@
       <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>9876543210</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="www.google.com"/>
     <hyperlink ref="K2" r:id="rId2" display="Coolshiv@facebook.com"/>
+    <hyperlink ref="O2" r:id="rId3" display="Coolshiv@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
instagram field added into staging branch
</commit_message>
<xml_diff>
--- a/public/invitee_sample.xlsx
+++ b/public/invitee_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="176" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="170" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>email</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>linkedin_link</t>
+  </si>
+  <si>
+    <t>instagram</t>
   </si>
   <si>
     <t>password</t>
@@ -110,7 +113,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -138,6 +141,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -182,12 +191,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -208,10 +221,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -280,58 +293,65 @@
       <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>9876543210</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="www.google.com"/>
     <hyperlink ref="K2" r:id="rId2" display="Coolshiv@facebook.com"/>
+    <hyperlink ref="O2" r:id="rId3" display="Coolshiv@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>